<commit_message>
lights move and work now, milestone 2 push
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="89">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>https://www.models-resource.com/nintendo_64/pokemonsnap/model/4943/</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>https://www.models-resource.com/pc_computer/zootycoon2/model/17846/</t>
   </si>
 </sst>
 </file>
@@ -926,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1065,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E71,"=III",G4:G71) + SUMIF(E73:E74, "X",B73:B74) &gt; 18, 18, SUMIF(E4:E71,"=III",G4:G71) + SUMIF(E73:E74, "X",B73:B74))</f>
@@ -1067,11 +1073,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G71) + SUMIF(C73:C74, "X",B73:B74) + SUMIF(D73:D74, "X",B73:B74) + SUMIF(E73:E74, "X",B73:B74)</f>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1132,7 +1138,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74)  &gt; 18, SUMIF(E4:E71,"=I",G4:G71) + SUMIF(C73:C74, "X",B73:B74) - 18,0)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) &gt; 18, SUMIF(E4:E71,"=II",G4:G71) + SUMIF(D73:D74, "X",B73:B74) - 18,0)</f>
@@ -1204,11 +1210,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1265,11 +1271,11 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
@@ -1617,14 +1623,14 @@
         <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>85</v>
       </c>
       <c r="G26" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1703,11 +1709,15 @@
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
+      <c r="E29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G29" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -1728,11 +1738,15 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1753,11 +1767,15 @@
       <c r="D31" s="5">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G31" s="16">
         <f t="shared" ref="G31:G55" si="1" xml:space="preserve"> IF(EXACT(F31,"X"),IF(EXACT(E31,"I"),$B31,IF(EXACT(E31,"II"),$C31,IF(EXACT(E31,"III"),$D31,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2084,11 +2102,15 @@
       <c r="D46" s="5">
         <v>2</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G46" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
@@ -2109,11 +2131,15 @@
       <c r="D47" s="5">
         <v>3</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="3"/>
+      <c r="E47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G47" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2649,7 +2675,9 @@
       <c r="C73" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
@@ -2669,7 +2697,9 @@
       <c r="C74" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D74" s="3"/>
+      <c r="D74" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E74" s="3"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
@@ -2718,7 +2748,9 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
+      <c r="A79" s="12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="12"/>

</xml_diff>